<commit_message>
undo and export buttons added
</commit_message>
<xml_diff>
--- a/pivot.xlsx
+++ b/pivot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suryaganesan/vscode/ml/projects/reporter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1441563E-D9DD-7242-BCEB-62D0B92AF2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06DAEC2-E1EB-9A47-8F36-E8B02C0360A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -90,14 +90,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -457,14 +475,22 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>3746.7</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>